<commit_message>
fixed values in pokemon.csv, completed the AbilityMap with all abilities
</commit_message>
<xml_diff>
--- a/Pokemon/src/pokemon/data/pokemon_actual_values.xlsx
+++ b/Pokemon/src/pokemon/data/pokemon_actual_values.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9758B168-D488-4F8E-A368-3B545DCB4D4F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -3330,7 +3331,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3645,18 +3646,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z494"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A286" workbookViewId="0">
-      <selection activeCell="F298" sqref="F298"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3956,16 +3957,16 @@
         <v>80</v>
       </c>
       <c r="P4" s="1">
+        <v>82</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>83</v>
+      </c>
+      <c r="R4" s="1">
         <v>100</v>
       </c>
-      <c r="Q4" s="1">
-        <v>123</v>
-      </c>
-      <c r="R4" s="1">
-        <v>122</v>
-      </c>
       <c r="S4" s="1">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="T4" s="1">
         <v>80</v>
@@ -4196,16 +4197,16 @@
         <v>78</v>
       </c>
       <c r="P7" s="1">
-        <v>104</v>
+        <v>84</v>
       </c>
       <c r="Q7" s="1">
         <v>78</v>
       </c>
       <c r="R7" s="1">
-        <v>159</v>
+        <v>109</v>
       </c>
       <c r="S7" s="1">
-        <v>115</v>
+        <v>85</v>
       </c>
       <c r="T7" s="1">
         <v>100</v>
@@ -4436,16 +4437,16 @@
         <v>79</v>
       </c>
       <c r="P10" s="1">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="Q10" s="1">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="R10" s="1">
-        <v>135</v>
+        <v>85</v>
       </c>
       <c r="S10" s="1">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="T10" s="1">
         <v>78</v>
@@ -4682,7 +4683,7 @@
         <v>50</v>
       </c>
       <c r="R13" s="1">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="S13" s="1">
         <v>80</v>
@@ -4916,19 +4917,19 @@
         <v>65</v>
       </c>
       <c r="P16" s="1">
-        <v>150</v>
+        <v>80</v>
       </c>
       <c r="Q16" s="1">
         <v>40</v>
       </c>
       <c r="R16" s="1">
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="S16" s="1">
         <v>80</v>
       </c>
       <c r="T16" s="1">
-        <v>145</v>
+        <v>75</v>
       </c>
       <c r="U16" s="1">
         <v>0</v>
@@ -5159,16 +5160,16 @@
         <v>80</v>
       </c>
       <c r="Q19" s="1">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="R19" s="1">
-        <v>135</v>
+        <v>70</v>
       </c>
       <c r="S19" s="1">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="T19" s="1">
-        <v>121</v>
+        <v>91</v>
       </c>
       <c r="U19" s="1">
         <v>0</v>
@@ -5313,22 +5314,22 @@
         <v>0</v>
       </c>
       <c r="O21" s="1">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="P21" s="1">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="Q21" s="1">
+        <v>60</v>
+      </c>
+      <c r="R21" s="1">
+        <v>50</v>
+      </c>
+      <c r="S21" s="1">
         <v>70</v>
       </c>
-      <c r="R21" s="1">
-        <v>40</v>
-      </c>
-      <c r="S21" s="1">
-        <v>80</v>
-      </c>
       <c r="T21" s="1">
-        <v>77</v>
+        <v>97</v>
       </c>
       <c r="U21" s="1">
         <v>0</v>
@@ -5636,7 +5637,7 @@
         <v>60</v>
       </c>
       <c r="P25" s="1">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="Q25" s="1">
         <v>69</v>
@@ -5719,13 +5720,13 @@
         <v>55</v>
       </c>
       <c r="Q26" s="1">
+        <v>30</v>
+      </c>
+      <c r="R26" s="1">
+        <v>50</v>
+      </c>
+      <c r="S26" s="1">
         <v>40</v>
-      </c>
-      <c r="R26" s="1">
-        <v>50</v>
-      </c>
-      <c r="S26" s="1">
-        <v>50</v>
       </c>
       <c r="T26" s="1">
         <v>90</v>
@@ -5796,19 +5797,19 @@
         <v>60</v>
       </c>
       <c r="P27" s="1">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="Q27" s="1">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="R27" s="1">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="S27" s="1">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="T27" s="1">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="U27" s="1">
         <v>0</v>
@@ -5879,13 +5880,13 @@
         <v>75</v>
       </c>
       <c r="Q28" s="1">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="R28" s="1">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="S28" s="1">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="T28" s="1">
         <v>40</v>
@@ -5959,13 +5960,13 @@
         <v>100</v>
       </c>
       <c r="Q29" s="1">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="R29" s="1">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="S29" s="1">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="T29" s="1">
         <v>65</v>
@@ -6196,7 +6197,7 @@
         <v>90</v>
       </c>
       <c r="P32" s="1">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="Q32" s="1">
         <v>87</v>
@@ -6436,7 +6437,7 @@
         <v>81</v>
       </c>
       <c r="P35" s="1">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="Q35" s="1">
         <v>77</v>
@@ -6602,7 +6603,7 @@
         <v>73</v>
       </c>
       <c r="R37" s="1">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="S37" s="1">
         <v>90</v>
@@ -6756,7 +6757,7 @@
         <v>73</v>
       </c>
       <c r="P39" s="1">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="Q39" s="1">
         <v>75</v>
@@ -6768,7 +6769,7 @@
         <v>100</v>
       </c>
       <c r="T39" s="1">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="U39" s="1">
         <v>0</v>
@@ -6922,7 +6923,7 @@
         <v>45</v>
       </c>
       <c r="R41" s="1">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="S41" s="1">
         <v>50</v>
@@ -7322,7 +7323,7 @@
         <v>85</v>
       </c>
       <c r="R46" s="1">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="S46" s="1">
         <v>90</v>
@@ -7719,7 +7720,7 @@
         <v>55</v>
       </c>
       <c r="Q51" s="1">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="R51" s="1">
         <v>35</v>
@@ -7728,7 +7729,7 @@
         <v>45</v>
       </c>
       <c r="T51" s="1">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="U51" s="1">
         <v>0</v>
@@ -7796,10 +7797,10 @@
         <v>35</v>
       </c>
       <c r="P52" s="1">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="Q52" s="1">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="R52" s="1">
         <v>50</v>
@@ -7808,7 +7809,7 @@
         <v>70</v>
       </c>
       <c r="T52" s="1">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="U52" s="1">
         <v>0</v>
@@ -7876,13 +7877,13 @@
         <v>40</v>
       </c>
       <c r="P53" s="1">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="Q53" s="1">
         <v>35</v>
       </c>
       <c r="R53" s="1">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="S53" s="1">
         <v>40</v>
@@ -7956,13 +7957,13 @@
         <v>65</v>
       </c>
       <c r="P54" s="1">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="Q54" s="1">
         <v>60</v>
       </c>
       <c r="R54" s="1">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="S54" s="1">
         <v>65</v>
@@ -8676,7 +8677,7 @@
         <v>90</v>
       </c>
       <c r="P63" s="1">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="Q63" s="1">
         <v>95</v>
@@ -8919,16 +8920,16 @@
         <v>50</v>
       </c>
       <c r="Q66" s="1">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="R66" s="1">
-        <v>175</v>
+        <v>135</v>
       </c>
       <c r="S66" s="1">
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="T66" s="1">
-        <v>150</v>
+        <v>120</v>
       </c>
       <c r="U66" s="1">
         <v>0</v>
@@ -9405,7 +9406,7 @@
         <v>100</v>
       </c>
       <c r="S72" s="1">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="T72" s="1">
         <v>70</v>
@@ -9796,7 +9797,7 @@
         <v>80</v>
       </c>
       <c r="P77" s="1">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="Q77" s="1">
         <v>130</v>
@@ -10119,10 +10120,10 @@
         <v>75</v>
       </c>
       <c r="Q81" s="1">
-        <v>180</v>
+        <v>110</v>
       </c>
       <c r="R81" s="1">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="S81" s="1">
         <v>80</v>
@@ -10356,7 +10357,7 @@
         <v>52</v>
       </c>
       <c r="P84" s="1">
-        <v>90</v>
+        <v>65</v>
       </c>
       <c r="Q84" s="1">
         <v>55</v>
@@ -10528,7 +10529,7 @@
         <v>60</v>
       </c>
       <c r="T86" s="1">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="U86" s="1">
         <v>0</v>
@@ -11239,16 +11240,16 @@
         <v>65</v>
       </c>
       <c r="Q95" s="1">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="R95" s="1">
-        <v>170</v>
+        <v>130</v>
       </c>
       <c r="S95" s="1">
-        <v>95</v>
+        <v>75</v>
       </c>
       <c r="T95" s="1">
-        <v>130</v>
+        <v>110</v>
       </c>
       <c r="U95" s="1">
         <v>0</v>
@@ -11808,7 +11809,7 @@
         <v>80</v>
       </c>
       <c r="T102" s="1">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="U102" s="1">
         <v>0</v>
@@ -11956,7 +11957,7 @@
         <v>95</v>
       </c>
       <c r="P104" s="1">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="Q104" s="1">
         <v>85</v>
@@ -11965,10 +11966,10 @@
         <v>125</v>
       </c>
       <c r="S104" s="1">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="T104" s="1">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="U104" s="1">
         <v>0</v>
@@ -12916,19 +12917,19 @@
         <v>105</v>
       </c>
       <c r="P116" s="1">
-        <v>125</v>
+        <v>95</v>
       </c>
       <c r="Q116" s="1">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="R116" s="1">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="S116" s="1">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="T116" s="1">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="U116" s="1">
         <v>2</v>
@@ -13876,19 +13877,19 @@
         <v>65</v>
       </c>
       <c r="P128" s="1">
-        <v>155</v>
+        <v>125</v>
       </c>
       <c r="Q128" s="1">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="R128" s="1">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="S128" s="1">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="T128" s="1">
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="U128" s="1">
         <v>0</v>
@@ -14116,16 +14117,16 @@
         <v>95</v>
       </c>
       <c r="P131" s="1">
-        <v>155</v>
+        <v>125</v>
       </c>
       <c r="Q131" s="1">
-        <v>109</v>
+        <v>79</v>
       </c>
       <c r="R131" s="1">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="S131" s="1">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="T131" s="1">
         <v>81</v>
@@ -15076,19 +15077,19 @@
         <v>80</v>
       </c>
       <c r="P143" s="1">
-        <v>135</v>
+        <v>105</v>
       </c>
       <c r="Q143" s="1">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="R143" s="1">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="S143" s="1">
-        <v>95</v>
+        <v>75</v>
       </c>
       <c r="T143" s="1">
-        <v>150</v>
+        <v>130</v>
       </c>
       <c r="U143" s="1">
         <v>0</v>
@@ -15716,19 +15717,19 @@
         <v>106</v>
       </c>
       <c r="P151" s="1">
-        <v>150</v>
+        <v>110</v>
       </c>
       <c r="Q151" s="1">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="R151" s="1">
-        <v>194</v>
+        <v>154</v>
       </c>
       <c r="S151" s="1">
-        <v>120</v>
+        <v>90</v>
       </c>
       <c r="T151" s="1">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="U151" s="1">
         <v>0</v>
@@ -16842,7 +16843,7 @@
         <v>50</v>
       </c>
       <c r="R165" s="1">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="S165" s="1">
         <v>96</v>
@@ -17165,7 +17166,7 @@
         <v>60</v>
       </c>
       <c r="S169" s="1">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="T169" s="1">
         <v>40</v>
@@ -18196,19 +18197,19 @@
         <v>90</v>
       </c>
       <c r="P182" s="1">
-        <v>95</v>
+        <v>75</v>
       </c>
       <c r="Q182" s="1">
-        <v>105</v>
+        <v>75</v>
       </c>
       <c r="R182" s="1">
-        <v>165</v>
+        <v>115</v>
       </c>
       <c r="S182" s="1">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="T182" s="1">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="U182" s="1">
         <v>0</v>
@@ -18279,7 +18280,7 @@
         <v>80</v>
       </c>
       <c r="Q183" s="1">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="R183" s="1">
         <v>90</v>
@@ -18442,7 +18443,7 @@
         <v>80</v>
       </c>
       <c r="R185" s="1">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="S185" s="1">
         <v>80</v>
@@ -18845,7 +18846,7 @@
         <v>55</v>
       </c>
       <c r="S190" s="1">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="T190" s="1">
         <v>110</v>
@@ -20356,16 +20357,16 @@
         <v>75</v>
       </c>
       <c r="P209" s="1">
-        <v>125</v>
+        <v>85</v>
       </c>
       <c r="Q209" s="1">
-        <v>230</v>
+        <v>200</v>
       </c>
       <c r="R209" s="1">
         <v>55</v>
       </c>
       <c r="S209" s="1">
-        <v>95</v>
+        <v>65</v>
       </c>
       <c r="T209" s="1">
         <v>30</v>
@@ -20599,7 +20600,7 @@
         <v>95</v>
       </c>
       <c r="Q212" s="1">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="R212" s="1">
         <v>55</v>
@@ -20676,19 +20677,19 @@
         <v>70</v>
       </c>
       <c r="P213" s="1">
-        <v>150</v>
+        <v>130</v>
       </c>
       <c r="Q213" s="1">
-        <v>140</v>
+        <v>100</v>
       </c>
       <c r="R213" s="1">
+        <v>55</v>
+      </c>
+      <c r="S213" s="1">
+        <v>80</v>
+      </c>
+      <c r="T213" s="1">
         <v>65</v>
-      </c>
-      <c r="S213" s="1">
-        <v>100</v>
-      </c>
-      <c r="T213" s="1">
-        <v>75</v>
       </c>
       <c r="U213" s="1">
         <v>0</v>
@@ -20836,19 +20837,19 @@
         <v>80</v>
       </c>
       <c r="P215" s="1">
-        <v>185</v>
+        <v>125</v>
       </c>
       <c r="Q215" s="1">
-        <v>115</v>
+        <v>75</v>
       </c>
       <c r="R215" s="1">
         <v>40</v>
       </c>
       <c r="S215" s="1">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="T215" s="1">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="U215" s="1">
         <v>0</v>
@@ -21233,7 +21234,7 @@
         <v>0</v>
       </c>
       <c r="O220" s="1">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="P220" s="1">
         <v>50</v>
@@ -21242,7 +21243,7 @@
         <v>120</v>
       </c>
       <c r="R220" s="1">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="S220" s="1">
         <v>80</v>
@@ -21473,19 +21474,19 @@
         <v>0</v>
       </c>
       <c r="O223" s="1">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="P223" s="1">
         <v>55</v>
       </c>
       <c r="Q223" s="1">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="R223" s="1">
         <v>65</v>
       </c>
       <c r="S223" s="1">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="T223" s="1">
         <v>35</v>
@@ -21793,7 +21794,7 @@
         <v>0</v>
       </c>
       <c r="O227" s="1">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="P227" s="1">
         <v>40</v>
@@ -22039,16 +22040,16 @@
         <v>90</v>
       </c>
       <c r="Q230" s="1">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="R230" s="1">
-        <v>140</v>
+        <v>110</v>
       </c>
       <c r="S230" s="1">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="T230" s="1">
-        <v>115</v>
+        <v>95</v>
       </c>
       <c r="U230" s="1">
         <v>0</v>
@@ -23556,19 +23557,19 @@
         <v>100</v>
       </c>
       <c r="P249" s="1">
-        <v>164</v>
+        <v>134</v>
       </c>
       <c r="Q249" s="1">
-        <v>150</v>
+        <v>110</v>
       </c>
       <c r="R249" s="1">
         <v>95</v>
       </c>
       <c r="S249" s="1">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="T249" s="1">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="U249" s="1">
         <v>0</v>
@@ -24036,19 +24037,19 @@
         <v>70</v>
       </c>
       <c r="P255" s="1">
-        <v>110</v>
+        <v>85</v>
       </c>
       <c r="Q255" s="1">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="R255" s="1">
-        <v>145</v>
+        <v>105</v>
       </c>
       <c r="S255" s="1">
         <v>85</v>
       </c>
       <c r="T255" s="1">
-        <v>145</v>
+        <v>120</v>
       </c>
       <c r="U255" s="1">
         <v>0</v>
@@ -24276,19 +24277,19 @@
         <v>80</v>
       </c>
       <c r="P258" s="1">
-        <v>160</v>
+        <v>120</v>
       </c>
       <c r="Q258" s="1">
+        <v>70</v>
+      </c>
+      <c r="R258" s="1">
+        <v>110</v>
+      </c>
+      <c r="S258" s="1">
+        <v>70</v>
+      </c>
+      <c r="T258" s="1">
         <v>80</v>
-      </c>
-      <c r="R258" s="1">
-        <v>130</v>
-      </c>
-      <c r="S258" s="1">
-        <v>80</v>
-      </c>
-      <c r="T258" s="1">
-        <v>100</v>
       </c>
       <c r="U258" s="1">
         <v>0</v>
@@ -24516,19 +24517,19 @@
         <v>100</v>
       </c>
       <c r="P261" s="1">
-        <v>150</v>
+        <v>110</v>
       </c>
       <c r="Q261" s="1">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="R261" s="1">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="S261" s="1">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="T261" s="1">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="U261" s="1">
         <v>0</v>
@@ -25082,7 +25083,7 @@
         <v>50</v>
       </c>
       <c r="R268" s="1">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="S268" s="1">
         <v>50</v>
@@ -25882,7 +25883,7 @@
         <v>60</v>
       </c>
       <c r="R278" s="1">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="S278" s="1">
         <v>50</v>
@@ -26042,7 +26043,7 @@
         <v>100</v>
       </c>
       <c r="R280" s="1">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="S280" s="1">
         <v>70</v>
@@ -26276,19 +26277,19 @@
         <v>68</v>
       </c>
       <c r="P283" s="1">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="Q283" s="1">
         <v>65</v>
       </c>
       <c r="R283" s="1">
-        <v>165</v>
+        <v>125</v>
       </c>
       <c r="S283" s="1">
-        <v>135</v>
+        <v>115</v>
       </c>
       <c r="T283" s="1">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="U283" s="1">
         <v>0</v>
@@ -26442,13 +26443,13 @@
         <v>62</v>
       </c>
       <c r="R285" s="1">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="S285" s="1">
         <v>82</v>
       </c>
       <c r="T285" s="1">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="U285" s="1">
         <v>0</v>
@@ -27325,7 +27326,7 @@
         <v>91</v>
       </c>
       <c r="S296" s="1">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="T296" s="1">
         <v>68</v>
@@ -27808,7 +27809,7 @@
         <v>55</v>
       </c>
       <c r="T302" s="1">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="U302" s="1">
         <v>1</v>
@@ -27876,19 +27877,19 @@
         <v>50</v>
       </c>
       <c r="P303" s="1">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="Q303" s="1">
-        <v>125</v>
+        <v>75</v>
       </c>
       <c r="R303" s="1">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="S303" s="1">
-        <v>115</v>
+        <v>65</v>
       </c>
       <c r="T303" s="1">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="U303" s="1">
         <v>0</v>
@@ -27956,16 +27957,16 @@
         <v>50</v>
       </c>
       <c r="P304" s="1">
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="Q304" s="1">
-        <v>125</v>
+        <v>85</v>
       </c>
       <c r="R304" s="1">
         <v>55</v>
       </c>
       <c r="S304" s="1">
-        <v>95</v>
+        <v>55</v>
       </c>
       <c r="T304" s="1">
         <v>50</v>
@@ -28196,16 +28197,16 @@
         <v>70</v>
       </c>
       <c r="P307" s="1">
-        <v>140</v>
+        <v>110</v>
       </c>
       <c r="Q307" s="1">
-        <v>230</v>
+        <v>180</v>
       </c>
       <c r="R307" s="1">
         <v>60</v>
       </c>
       <c r="S307" s="1">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="T307" s="1">
         <v>50</v>
@@ -28356,19 +28357,19 @@
         <v>60</v>
       </c>
       <c r="P309" s="1">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="Q309" s="1">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="R309" s="1">
+        <v>60</v>
+      </c>
+      <c r="S309" s="1">
+        <v>75</v>
+      </c>
+      <c r="T309" s="1">
         <v>80</v>
-      </c>
-      <c r="S309" s="1">
-        <v>85</v>
-      </c>
-      <c r="T309" s="1">
-        <v>100</v>
       </c>
       <c r="U309" s="1">
         <v>0</v>
@@ -28519,16 +28520,16 @@
         <v>75</v>
       </c>
       <c r="Q311" s="1">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="R311" s="1">
-        <v>135</v>
+        <v>105</v>
       </c>
       <c r="S311" s="1">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="T311" s="1">
-        <v>135</v>
+        <v>105</v>
       </c>
       <c r="U311" s="1">
         <v>0</v>
@@ -28759,13 +28760,13 @@
         <v>73</v>
       </c>
       <c r="Q314" s="1">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="R314" s="1">
         <v>47</v>
       </c>
       <c r="S314" s="1">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="T314" s="1">
         <v>85</v>
@@ -28839,13 +28840,13 @@
         <v>47</v>
       </c>
       <c r="Q315" s="1">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="R315" s="1">
         <v>73</v>
       </c>
       <c r="S315" s="1">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="T315" s="1">
         <v>85</v>
@@ -29236,19 +29237,19 @@
         <v>70</v>
       </c>
       <c r="P320" s="1">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="Q320" s="1">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="R320" s="1">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="S320" s="1">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="T320" s="1">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="U320" s="1">
         <v>0</v>
@@ -29556,19 +29557,19 @@
         <v>70</v>
       </c>
       <c r="P324" s="1">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="Q324" s="1">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="R324" s="1">
-        <v>145</v>
+        <v>105</v>
       </c>
       <c r="S324" s="1">
-        <v>105</v>
+        <v>75</v>
       </c>
       <c r="T324" s="1">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="U324" s="1">
         <v>0</v>
@@ -30436,13 +30437,13 @@
         <v>75</v>
       </c>
       <c r="P335" s="1">
-        <v>110</v>
+        <v>70</v>
       </c>
       <c r="Q335" s="1">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="R335" s="1">
-        <v>110</v>
+        <v>70</v>
       </c>
       <c r="S335" s="1">
         <v>105</v>
@@ -30673,7 +30674,7 @@
         <v>0</v>
       </c>
       <c r="O338" s="1">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="P338" s="1">
         <v>55</v>
@@ -30753,7 +30754,7 @@
         <v>0</v>
       </c>
       <c r="O339" s="1">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="P339" s="1">
         <v>95</v>
@@ -32036,19 +32037,19 @@
         <v>64</v>
       </c>
       <c r="P355" s="1">
-        <v>165</v>
+        <v>115</v>
       </c>
       <c r="Q355" s="1">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="R355" s="1">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="S355" s="1">
-        <v>83</v>
+        <v>63</v>
       </c>
       <c r="T355" s="1">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="U355" s="1">
         <v>0</v>
@@ -32353,19 +32354,19 @@
         <v>0</v>
       </c>
       <c r="O359" s="1">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="P359" s="1">
         <v>50</v>
       </c>
       <c r="Q359" s="1">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="R359" s="1">
         <v>95</v>
       </c>
       <c r="S359" s="1">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="T359" s="1">
         <v>65</v>
@@ -32436,19 +32437,19 @@
         <v>65</v>
       </c>
       <c r="P360" s="1">
-        <v>150</v>
+        <v>130</v>
       </c>
       <c r="Q360" s="1">
         <v>60</v>
       </c>
       <c r="R360" s="1">
-        <v>115</v>
+        <v>75</v>
       </c>
       <c r="S360" s="1">
         <v>60</v>
       </c>
       <c r="T360" s="1">
-        <v>115</v>
+        <v>75</v>
       </c>
       <c r="U360" s="1">
         <v>0</v>
@@ -32676,19 +32677,19 @@
         <v>80</v>
       </c>
       <c r="P363" s="1">
-        <v>120</v>
+        <v>80</v>
       </c>
       <c r="Q363" s="1">
         <v>80</v>
       </c>
       <c r="R363" s="1">
-        <v>120</v>
+        <v>80</v>
       </c>
       <c r="S363" s="1">
         <v>80</v>
       </c>
       <c r="T363" s="1">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="U363" s="1">
         <v>2</v>
@@ -33556,19 +33557,19 @@
         <v>95</v>
       </c>
       <c r="P374" s="1">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="Q374" s="1">
-        <v>130</v>
+        <v>80</v>
       </c>
       <c r="R374" s="1">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="S374" s="1">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="T374" s="1">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="U374" s="1">
         <v>0</v>
@@ -33796,19 +33797,19 @@
         <v>80</v>
       </c>
       <c r="P377" s="1">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="Q377" s="1">
-        <v>150</v>
+        <v>130</v>
       </c>
       <c r="R377" s="1">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="S377" s="1">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="T377" s="1">
-        <v>110</v>
+        <v>70</v>
       </c>
       <c r="U377" s="1">
         <v>0</v>
@@ -34116,16 +34117,16 @@
         <v>80</v>
       </c>
       <c r="P381" s="1">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="Q381" s="1">
-        <v>120</v>
+        <v>90</v>
       </c>
       <c r="R381" s="1">
-        <v>140</v>
+        <v>110</v>
       </c>
       <c r="S381" s="1">
-        <v>150</v>
+        <v>130</v>
       </c>
       <c r="T381" s="1">
         <v>110</v>
@@ -34196,16 +34197,16 @@
         <v>80</v>
       </c>
       <c r="P382" s="1">
+        <v>90</v>
+      </c>
+      <c r="Q382" s="1">
+        <v>80</v>
+      </c>
+      <c r="R382" s="1">
         <v>130</v>
       </c>
-      <c r="Q382" s="1">
-        <v>100</v>
-      </c>
-      <c r="R382" s="1">
-        <v>160</v>
-      </c>
       <c r="S382" s="1">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="T382" s="1">
         <v>110</v>
@@ -34276,16 +34277,16 @@
         <v>100</v>
       </c>
       <c r="P383" s="1">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="Q383" s="1">
         <v>90</v>
       </c>
       <c r="R383" s="1">
-        <v>180</v>
+        <v>150</v>
       </c>
       <c r="S383" s="1">
-        <v>160</v>
+        <v>140</v>
       </c>
       <c r="T383" s="1">
         <v>90</v>
@@ -34356,13 +34357,13 @@
         <v>100</v>
       </c>
       <c r="P384" s="1">
-        <v>180</v>
+        <v>150</v>
       </c>
       <c r="Q384" s="1">
-        <v>160</v>
+        <v>140</v>
       </c>
       <c r="R384" s="1">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="S384" s="1">
         <v>90</v>
@@ -34436,19 +34437,19 @@
         <v>105</v>
       </c>
       <c r="P385" s="1">
-        <v>180</v>
+        <v>150</v>
       </c>
       <c r="Q385" s="1">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="R385" s="1">
-        <v>180</v>
+        <v>150</v>
       </c>
       <c r="S385" s="1">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="T385" s="1">
-        <v>115</v>
+        <v>95</v>
       </c>
       <c r="U385" s="1">
         <v>0</v>
@@ -34596,19 +34597,19 @@
         <v>50</v>
       </c>
       <c r="P387" s="1">
-        <v>95</v>
+        <v>150</v>
       </c>
       <c r="Q387" s="1">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="R387" s="1">
-        <v>95</v>
+        <v>150</v>
       </c>
       <c r="S387" s="1">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="T387" s="1">
-        <v>180</v>
+        <v>150</v>
       </c>
       <c r="U387" s="1">
         <v>0</v>
@@ -35565,7 +35566,7 @@
         <v>50</v>
       </c>
       <c r="S399" s="1">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="T399" s="1">
         <v>100</v>
@@ -36279,7 +36280,7 @@
         <v>70</v>
       </c>
       <c r="Q408" s="1">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="R408" s="1">
         <v>125</v>
@@ -36756,16 +36757,16 @@
         <v>60</v>
       </c>
       <c r="P414" s="1">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="Q414" s="1">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="R414" s="1">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="S414" s="1">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="T414" s="1">
         <v>36</v>
@@ -37956,10 +37957,10 @@
         <v>65</v>
       </c>
       <c r="P429" s="1">
-        <v>136</v>
+        <v>76</v>
       </c>
       <c r="Q429" s="1">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="R429" s="1">
         <v>54</v>
@@ -37968,7 +37969,7 @@
         <v>96</v>
       </c>
       <c r="T429" s="1">
-        <v>135</v>
+        <v>105</v>
       </c>
       <c r="U429" s="1">
         <v>0</v>
@@ -39316,19 +39317,19 @@
         <v>108</v>
       </c>
       <c r="P446" s="1">
-        <v>170</v>
+        <v>130</v>
       </c>
       <c r="Q446" s="1">
-        <v>115</v>
+        <v>95</v>
       </c>
       <c r="R446" s="1">
-        <v>120</v>
+        <v>80</v>
       </c>
       <c r="S446" s="1">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="T446" s="1">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="U446" s="1">
         <v>0</v>
@@ -39556,19 +39557,19 @@
         <v>70</v>
       </c>
       <c r="P449" s="1">
-        <v>145</v>
+        <v>110</v>
       </c>
       <c r="Q449" s="1">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="R449" s="1">
-        <v>140</v>
+        <v>115</v>
       </c>
       <c r="S449" s="1">
         <v>70</v>
       </c>
       <c r="T449" s="1">
-        <v>112</v>
+        <v>90</v>
       </c>
       <c r="U449" s="1">
         <v>0</v>
@@ -40516,19 +40517,19 @@
         <v>90</v>
       </c>
       <c r="P461" s="1">
-        <v>132</v>
+        <v>92</v>
       </c>
       <c r="Q461" s="1">
-        <v>105</v>
+        <v>75</v>
       </c>
       <c r="R461" s="1">
-        <v>132</v>
+        <v>92</v>
       </c>
       <c r="S461" s="1">
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="T461" s="1">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="U461" s="1">
         <v>0</v>
@@ -41716,10 +41717,10 @@
         <v>68</v>
       </c>
       <c r="P476" s="1">
-        <v>165</v>
+        <v>125</v>
       </c>
       <c r="Q476" s="1">
-        <v>95</v>
+        <v>65</v>
       </c>
       <c r="R476" s="1">
         <v>65</v>
@@ -41728,7 +41729,7 @@
         <v>115</v>
       </c>
       <c r="T476" s="1">
-        <v>110</v>
+        <v>80</v>
       </c>
       <c r="U476" s="1">
         <v>0</v>
@@ -42036,19 +42037,19 @@
         <v>50</v>
       </c>
       <c r="P480" s="1">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="Q480" s="1">
-        <v>107</v>
+        <v>77</v>
       </c>
       <c r="R480" s="1">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="S480" s="1">
-        <v>107</v>
+        <v>77</v>
       </c>
       <c r="T480" s="1">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="U480" s="1">
         <v>0</v>
@@ -42676,16 +42677,16 @@
         <v>150</v>
       </c>
       <c r="P488" s="1">
+        <v>100</v>
+      </c>
+      <c r="Q488" s="1">
         <v>120</v>
       </c>
-      <c r="Q488" s="1">
+      <c r="R488" s="1">
         <v>100</v>
       </c>
-      <c r="R488" s="1">
+      <c r="S488" s="1">
         <v>120</v>
-      </c>
-      <c r="S488" s="1">
-        <v>100</v>
       </c>
       <c r="T488" s="1">
         <v>90</v>
@@ -43076,19 +43077,19 @@
         <v>100</v>
       </c>
       <c r="P493" s="1">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="Q493" s="1">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="R493" s="1">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="S493" s="1">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="T493" s="1">
-        <v>127</v>
+        <v>100</v>
       </c>
       <c r="U493" s="1">
         <v>3</v>

</xml_diff>